<commit_message>
Sprint backlog open for sprint meeting
</commit_message>
<xml_diff>
--- a/Backlogs/Product_Backlog.xlsx
+++ b/Backlogs/Product_Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ircur\OneDrive\Documents\Year2\2XB3\ParkThisCar\Backlogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="55DC29AC327B36D776E8DCF734128A3D99A09A66" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{414E911A-875A-41F4-93C6-7CEAA676B7F3}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="55DC29AC327B36D776E8DCF734128A3D99A09A66" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{4C8BD766-5C86-4459-BDAF-D34CFDF3E111}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" xr2:uid="{9F81BDF8-6A0A-44AB-BD16-A2CAC4981C78}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Proiority</t>
   </si>
@@ -63,9 +63,6 @@
     <t>By</t>
   </si>
   <si>
-    <t>Estimated Time</t>
-  </si>
-  <si>
     <t>Very High Priority</t>
   </si>
   <si>
@@ -100,6 +97,12 @@
   </si>
   <si>
     <t>Determine paid vs free parking spots</t>
+  </si>
+  <si>
+    <t>Implement coordinates class</t>
+  </si>
+  <si>
+    <t>Estimated Time (hr)</t>
   </si>
 </sst>
 </file>
@@ -174,22 +177,22 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -509,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA4F14F9-D138-4093-8675-02895CE18BE9}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -530,29 +533,29 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>300</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -560,10 +563,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>8</v>
@@ -574,132 +577,145 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C5">
-        <v>100</v>
-      </c>
-      <c r="L5" t="s">
-        <v>1</v>
-      </c>
-      <c r="M5" t="s">
-        <v>2</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>400</v>
+        <v>10</v>
       </c>
       <c r="L6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="A7">
+        <v>3.1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
       <c r="L7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8">
-        <v>200</v>
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="L8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="L11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C10">
-        <v>150</v>
-      </c>
-      <c r="L10" t="s">
-        <v>5</v>
-      </c>
-      <c r="M10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="L11" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="L12" t="s">
         <v>7</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M12" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12">
-        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13">
-        <v>70</v>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>